<commit_message>
FEATURE Added 3Face overview in instructions, adjusted CN instruction text, sizing
</commit_message>
<xml_diff>
--- a/0_Instructions.xlsx
+++ b/0_Instructions.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="260" documentId="13_ncr:1_{1C5A802C-9E12-9642-81BF-202D7BBFE009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE2707C2-BE21-AC42-8709-EA60757CB07B}"/>
+  <xr:revisionPtr revIDLastSave="332" documentId="13_ncr:1_{1C5A802C-9E12-9642-81BF-202D7BBFE009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91EEA07C-E309-4C90-88BF-FAB8A4A8CD46}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="6945" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="33">
   <si>
     <t>You will see different faces appear on the screen. Please carefully observe them.</t>
   </si>
@@ -85,18 +85,12 @@
     <t>Before we continue, feel free to take a break of 5-10 minutes.</t>
   </si>
   <si>
-    <t>当你看到下面的面孔时，请以最快的速度按下鼠标左键。</t>
-  </si>
-  <si>
     <t>请放松地坐在椅子上，并始终注视于屏幕。</t>
   </si>
   <si>
     <t>同样，你会看到屏幕上出现不同的面孔。请仔细观察它们。</t>
   </si>
   <si>
-    <t>一旦你准备好了，请按下'Continue'.</t>
-  </si>
-  <si>
     <t>在我们继续之前，请放松地休息5-10分钟.</t>
   </si>
   <si>
@@ -110,13 +104,28 @@
   </si>
   <si>
     <t>本阶段结束。请短暂休息一下，等待开启下一阶段的指令。</t>
+  </si>
+  <si>
+    <t>When you see any of the faces below, do nothing.</t>
+  </si>
+  <si>
+    <t>Stimuli/Raw_3Faces.BMP</t>
+  </si>
+  <si>
+    <t>当你看到下面的任何一张脸时，什么都不要做。</t>
+  </si>
+  <si>
+    <t>当你看到下面的脸时，以最快的速度按下空格。</t>
+  </si>
+  <si>
+    <t>一旦你准备好了，按空格</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,18 +149,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -170,8 +167,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="PingFang SC Regular"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="PingFang SC Regular"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="PingFang SC Regular"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="PingFang SC Regular"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -196,10 +216,25 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -209,61 +244,100 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -280,6 +354,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -547,247 +625,580 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2" zoomScale="373" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="17.7" x14ac:dyDescent="0.85"/>
   <cols>
-    <col min="1" max="1" width="33.33203125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="33.33203125" style="9" customWidth="1"/>
-    <col min="3" max="4" width="33.33203125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="30.33203125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="33.33203125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="25.5" style="5" customWidth="1"/>
-    <col min="8" max="8" width="39.1640625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="33.33203125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="16" style="5" customWidth="1"/>
-    <col min="11" max="11" width="26" style="5" customWidth="1"/>
-    <col min="12" max="16384" width="8.83203125" style="5"/>
+    <col min="1" max="1" width="33.3125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="33.3125" style="29" customWidth="1"/>
+    <col min="3" max="3" width="16.05078125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="33.3125" style="16" customWidth="1"/>
+    <col min="5" max="5" width="30.3125" style="29" customWidth="1"/>
+    <col min="6" max="6" width="12.62890625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="25.47265625" style="16" customWidth="1"/>
+    <col min="8" max="8" width="39.15625" style="29" customWidth="1"/>
+    <col min="9" max="9" width="15.15625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="23.89453125" style="16" customWidth="1"/>
+    <col min="11" max="11" width="26" style="29" customWidth="1"/>
+    <col min="12" max="16384" width="8.83984375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="3" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="14" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="A3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="F3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="G3" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="20"/>
+      <c r="K3" s="27"/>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="A4" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="22"/>
+      <c r="K4" s="31"/>
+    </row>
+    <row r="5" spans="1:11" s="14" customFormat="1" ht="46.8" x14ac:dyDescent="0.8">
+      <c r="A5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="B5" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="D5" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="20"/>
+      <c r="K5" s="27"/>
+    </row>
+    <row r="6" spans="1:11" s="1" customFormat="1" ht="59.05" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="A6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="D6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H6" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J6" s="22"/>
+      <c r="K6" s="31"/>
+    </row>
+    <row r="7" spans="1:11" s="12" customFormat="1" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="B7" s="27"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="27"/>
+      <c r="G7" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="15" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3"/>
-      <c r="K3"/>
-    </row>
-    <row r="4" spans="1:11" s="4" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-    </row>
-    <row r="5" spans="1:11" s="15" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5"/>
-      <c r="K5"/>
-    </row>
-    <row r="6" spans="1:11" s="4" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
-      <c r="F6"/>
-      <c r="G6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-    </row>
-    <row r="7" spans="1:11" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:11" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:11" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:11" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:11" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:11" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:11" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:11" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:11" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:11" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="17" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="18" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="19" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="20" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="21" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="22" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="23" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="24" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="26" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="27" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="28" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="29" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="30" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="31" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="32" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="33" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="34" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="35" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="36" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="37" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="38" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="39" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="40" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="41" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="42" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="43" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="44" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="45" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="27"/>
+    </row>
+    <row r="8" spans="1:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+      <c r="B8" s="28"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="28"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="28"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="28"/>
+    </row>
+    <row r="9" spans="1:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+      <c r="B9" s="28"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="28"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="28"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="28"/>
+    </row>
+    <row r="10" spans="1:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+      <c r="B10" s="28"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="28"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="28"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="28"/>
+    </row>
+    <row r="11" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.85">
+      <c r="B11" s="28"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="28"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="29"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="28"/>
+    </row>
+    <row r="12" spans="1:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+      <c r="B12" s="28"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="28"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="28"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="28"/>
+    </row>
+    <row r="13" spans="1:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+      <c r="B13" s="28"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="28"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="28"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="28"/>
+    </row>
+    <row r="14" spans="1:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+      <c r="B14" s="28"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="28"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="28"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="28"/>
+    </row>
+    <row r="15" spans="1:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+      <c r="B15" s="28"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="28"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="28"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="28"/>
+    </row>
+    <row r="16" spans="1:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+      <c r="B16" s="28"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="28"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="28"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="28"/>
+    </row>
+    <row r="17" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+      <c r="B17" s="28"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="28"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="28"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="28"/>
+    </row>
+    <row r="18" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+      <c r="B18" s="28"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="28"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="28"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="28"/>
+    </row>
+    <row r="19" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+      <c r="B19" s="28"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="28"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="28"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="28"/>
+    </row>
+    <row r="20" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+      <c r="B20" s="28"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="28"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="28"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="28"/>
+    </row>
+    <row r="21" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+      <c r="B21" s="28"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="28"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="28"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="28"/>
+    </row>
+    <row r="22" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+      <c r="B22" s="28"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="28"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="28"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="28"/>
+    </row>
+    <row r="23" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+      <c r="B23" s="28"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="28"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="28"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="28"/>
+    </row>
+    <row r="24" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+      <c r="B24" s="28"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="28"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="28"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="28"/>
+    </row>
+    <row r="25" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+      <c r="B25" s="28"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="28"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="28"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="28"/>
+    </row>
+    <row r="26" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+      <c r="B26" s="28"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="28"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="28"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="28"/>
+    </row>
+    <row r="27" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+      <c r="B27" s="28"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="28"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="28"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="28"/>
+    </row>
+    <row r="28" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+      <c r="B28" s="28"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="28"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="28"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="28"/>
+    </row>
+    <row r="29" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+      <c r="B29" s="28"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="28"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="28"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="28"/>
+    </row>
+    <row r="30" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+      <c r="B30" s="28"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="28"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="28"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="28"/>
+    </row>
+    <row r="31" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+      <c r="B31" s="28"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="28"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="28"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="28"/>
+    </row>
+    <row r="32" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+      <c r="B32" s="28"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="28"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="28"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="28"/>
+    </row>
+    <row r="33" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+      <c r="B33" s="28"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="28"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="28"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="28"/>
+    </row>
+    <row r="34" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+      <c r="B34" s="28"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="28"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="28"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="28"/>
+    </row>
+    <row r="35" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+      <c r="B35" s="28"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="28"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="28"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="28"/>
+    </row>
+    <row r="36" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+      <c r="B36" s="28"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="28"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="28"/>
+      <c r="J36" s="15"/>
+      <c r="K36" s="28"/>
+    </row>
+    <row r="37" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+      <c r="B37" s="28"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="28"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="28"/>
+      <c r="J37" s="15"/>
+      <c r="K37" s="28"/>
+    </row>
+    <row r="38" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+      <c r="B38" s="28"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="28"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="28"/>
+      <c r="J38" s="15"/>
+      <c r="K38" s="28"/>
+    </row>
+    <row r="39" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+      <c r="B39" s="28"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="28"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="28"/>
+      <c r="J39" s="15"/>
+      <c r="K39" s="28"/>
+    </row>
+    <row r="40" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+      <c r="B40" s="28"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="28"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="28"/>
+      <c r="J40" s="15"/>
+      <c r="K40" s="28"/>
+    </row>
+    <row r="41" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+      <c r="B41" s="28"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="28"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="28"/>
+      <c r="J41" s="15"/>
+      <c r="K41" s="28"/>
+    </row>
+    <row r="42" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+      <c r="B42" s="28"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="28"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="28"/>
+      <c r="J42" s="15"/>
+      <c r="K42" s="28"/>
+    </row>
+    <row r="43" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+      <c r="B43" s="28"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="28"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="28"/>
+      <c r="J43" s="15"/>
+      <c r="K43" s="28"/>
+    </row>
+    <row r="44" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+      <c r="B44" s="28"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="28"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="28"/>
+      <c r="J44" s="15"/>
+      <c r="K44" s="28"/>
+    </row>
+    <row r="45" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+      <c r="B45" s="28"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="28"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="28"/>
+      <c r="J45" s="15"/>
+      <c r="K45" s="28"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
BUG Improved CN Instructions
</commit_message>
<xml_diff>
--- a/0_Instructions.xlsx
+++ b/0_Instructions.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="332" documentId="13_ncr:1_{1C5A802C-9E12-9642-81BF-202D7BBFE009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91EEA07C-E309-4C90-88BF-FAB8A4A8CD46}"/>
+  <xr:revisionPtr revIDLastSave="338" documentId="13_ncr:1_{1C5A802C-9E12-9642-81BF-202D7BBFE009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9381E74F-0363-42A2-82A4-50836C312F19}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="6945" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -85,9 +85,6 @@
     <t>Before we continue, feel free to take a break of 5-10 minutes.</t>
   </si>
   <si>
-    <t>请放松地坐在椅子上，并始终注视于屏幕。</t>
-  </si>
-  <si>
     <t>同样，你会看到屏幕上出现不同的面孔。请仔细观察它们。</t>
   </si>
   <si>
@@ -112,20 +109,23 @@
     <t>Stimuli/Raw_3Faces.BMP</t>
   </si>
   <si>
-    <t>当你看到下面的任何一张脸时，什么都不要做。</t>
-  </si>
-  <si>
-    <t>当你看到下面的脸时，以最快的速度按下空格。</t>
-  </si>
-  <si>
     <t>一旦你准备好了，按空格</t>
+  </si>
+  <si>
+    <t>当你看到下面的面孔时，以最快的速度按下空格。</t>
+  </si>
+  <si>
+    <t>当你看到下面的任何一张面孔时，什么都不要做。</t>
+  </si>
+  <si>
+    <t>请放松地坐在椅子上，并始终注视屏幕。</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -625,27 +625,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="17.7" x14ac:dyDescent="0.85"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="33.3125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="33.3125" style="29" customWidth="1"/>
-    <col min="3" max="3" width="16.05078125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="33.3125" style="16" customWidth="1"/>
-    <col min="5" max="5" width="30.3125" style="29" customWidth="1"/>
-    <col min="6" max="6" width="12.62890625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="25.47265625" style="16" customWidth="1"/>
-    <col min="8" max="8" width="39.15625" style="29" customWidth="1"/>
-    <col min="9" max="9" width="15.15625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="23.89453125" style="16" customWidth="1"/>
+    <col min="1" max="1" width="33.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" style="29" customWidth="1"/>
+    <col min="3" max="3" width="16" style="3" customWidth="1"/>
+    <col min="4" max="4" width="33.28515625" style="16" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" style="29" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="25.42578125" style="16" customWidth="1"/>
+    <col min="8" max="8" width="39.140625" style="29" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="23.85546875" style="16" customWidth="1"/>
     <col min="11" max="11" width="26" style="29" customWidth="1"/>
-    <col min="12" max="16384" width="8.83984375" style="3"/>
+    <col min="12" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="36.6" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="37.5">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -680,42 +680,42 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="60" customHeight="1">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="23" t="s">
         <v>26</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>27</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>18</v>
       </c>
       <c r="G2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="30" t="s">
         <v>26</v>
-      </c>
-      <c r="H2" s="30" t="s">
-        <v>27</v>
       </c>
       <c r="I2" s="19" t="s">
         <v>18</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K2" s="23" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="14" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.8">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="14" customFormat="1" ht="84" customHeight="1">
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
@@ -729,7 +729,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>18</v>
@@ -738,7 +738,7 @@
         <v>20</v>
       </c>
       <c r="H3" s="26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I3" s="8" t="s">
         <v>18</v>
@@ -746,12 +746,12 @@
       <c r="J3" s="20"/>
       <c r="K3" s="27"/>
     </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="4" spans="1:11" s="1" customFormat="1" ht="48" customHeight="1">
       <c r="A4" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>15</v>
@@ -760,7 +760,7 @@
         <v>19</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F4" s="19" t="s">
         <v>15</v>
@@ -769,7 +769,7 @@
         <v>12</v>
       </c>
       <c r="H4" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I4" s="19" t="s">
         <v>18</v>
@@ -777,30 +777,30 @@
       <c r="J4" s="22"/>
       <c r="K4" s="31"/>
     </row>
-    <row r="5" spans="1:11" s="14" customFormat="1" ht="46.8" x14ac:dyDescent="0.8">
+    <row r="5" spans="1:11" s="14" customFormat="1" ht="63">
       <c r="A5" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>29</v>
-      </c>
       <c r="D5" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="10" t="s">
         <v>28</v>
-      </c>
-      <c r="E5" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>29</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>19</v>
       </c>
       <c r="H5" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I5" s="8" t="s">
         <v>15</v>
@@ -808,12 +808,12 @@
       <c r="J5" s="20"/>
       <c r="K5" s="27"/>
     </row>
-    <row r="6" spans="1:11" s="1" customFormat="1" ht="59.05" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="6" spans="1:11" s="1" customFormat="1" ht="59.1" customHeight="1">
       <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C6" s="19" t="s">
         <v>18</v>
@@ -822,24 +822,24 @@
         <v>13</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F6" s="19" t="s">
         <v>18</v>
       </c>
       <c r="G6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="H6" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="J6" s="22"/>
       <c r="K6" s="31"/>
     </row>
-    <row r="7" spans="1:11" s="12" customFormat="1" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="7" spans="1:11" s="12" customFormat="1" ht="69.599999999999994" customHeight="1">
       <c r="B7" s="27"/>
       <c r="D7" s="20"/>
       <c r="E7" s="27"/>
@@ -847,7 +847,7 @@
         <v>13</v>
       </c>
       <c r="H7" s="26" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I7" s="10" t="s">
         <v>18</v>
@@ -855,7 +855,7 @@
       <c r="J7" s="20"/>
       <c r="K7" s="27"/>
     </row>
-    <row r="8" spans="1:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+    <row r="8" spans="1:11" s="7" customFormat="1" ht="15">
       <c r="B8" s="28"/>
       <c r="D8" s="15"/>
       <c r="E8" s="28"/>
@@ -864,7 +864,7 @@
       <c r="J8" s="15"/>
       <c r="K8" s="28"/>
     </row>
-    <row r="9" spans="1:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+    <row r="9" spans="1:11" s="7" customFormat="1" ht="15">
       <c r="B9" s="28"/>
       <c r="D9" s="15"/>
       <c r="E9" s="28"/>
@@ -873,7 +873,7 @@
       <c r="J9" s="15"/>
       <c r="K9" s="28"/>
     </row>
-    <row r="10" spans="1:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+    <row r="10" spans="1:11" s="7" customFormat="1" ht="15">
       <c r="B10" s="28"/>
       <c r="D10" s="15"/>
       <c r="E10" s="28"/>
@@ -882,7 +882,7 @@
       <c r="J10" s="15"/>
       <c r="K10" s="28"/>
     </row>
-    <row r="11" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.85">
+    <row r="11" spans="1:11" s="7" customFormat="1">
       <c r="B11" s="28"/>
       <c r="D11" s="15"/>
       <c r="E11" s="28"/>
@@ -891,7 +891,7 @@
       <c r="J11" s="15"/>
       <c r="K11" s="28"/>
     </row>
-    <row r="12" spans="1:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+    <row r="12" spans="1:11" s="7" customFormat="1" ht="15">
       <c r="B12" s="28"/>
       <c r="D12" s="15"/>
       <c r="E12" s="28"/>
@@ -900,7 +900,7 @@
       <c r="J12" s="15"/>
       <c r="K12" s="28"/>
     </row>
-    <row r="13" spans="1:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+    <row r="13" spans="1:11" s="7" customFormat="1" ht="15">
       <c r="B13" s="28"/>
       <c r="D13" s="15"/>
       <c r="E13" s="28"/>
@@ -909,7 +909,7 @@
       <c r="J13" s="15"/>
       <c r="K13" s="28"/>
     </row>
-    <row r="14" spans="1:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+    <row r="14" spans="1:11" s="7" customFormat="1" ht="15">
       <c r="B14" s="28"/>
       <c r="D14" s="15"/>
       <c r="E14" s="28"/>
@@ -918,7 +918,7 @@
       <c r="J14" s="15"/>
       <c r="K14" s="28"/>
     </row>
-    <row r="15" spans="1:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+    <row r="15" spans="1:11" s="7" customFormat="1" ht="15">
       <c r="B15" s="28"/>
       <c r="D15" s="15"/>
       <c r="E15" s="28"/>
@@ -927,7 +927,7 @@
       <c r="J15" s="15"/>
       <c r="K15" s="28"/>
     </row>
-    <row r="16" spans="1:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+    <row r="16" spans="1:11" s="7" customFormat="1" ht="15">
       <c r="B16" s="28"/>
       <c r="D16" s="15"/>
       <c r="E16" s="28"/>
@@ -936,7 +936,7 @@
       <c r="J16" s="15"/>
       <c r="K16" s="28"/>
     </row>
-    <row r="17" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+    <row r="17" spans="2:11" s="7" customFormat="1" ht="15">
       <c r="B17" s="28"/>
       <c r="D17" s="15"/>
       <c r="E17" s="28"/>
@@ -945,7 +945,7 @@
       <c r="J17" s="15"/>
       <c r="K17" s="28"/>
     </row>
-    <row r="18" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+    <row r="18" spans="2:11" s="7" customFormat="1" ht="15">
       <c r="B18" s="28"/>
       <c r="D18" s="15"/>
       <c r="E18" s="28"/>
@@ -954,7 +954,7 @@
       <c r="J18" s="15"/>
       <c r="K18" s="28"/>
     </row>
-    <row r="19" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+    <row r="19" spans="2:11" s="7" customFormat="1" ht="15">
       <c r="B19" s="28"/>
       <c r="D19" s="15"/>
       <c r="E19" s="28"/>
@@ -963,7 +963,7 @@
       <c r="J19" s="15"/>
       <c r="K19" s="28"/>
     </row>
-    <row r="20" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+    <row r="20" spans="2:11" s="7" customFormat="1" ht="15">
       <c r="B20" s="28"/>
       <c r="D20" s="15"/>
       <c r="E20" s="28"/>
@@ -972,7 +972,7 @@
       <c r="J20" s="15"/>
       <c r="K20" s="28"/>
     </row>
-    <row r="21" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+    <row r="21" spans="2:11" s="7" customFormat="1" ht="15">
       <c r="B21" s="28"/>
       <c r="D21" s="15"/>
       <c r="E21" s="28"/>
@@ -981,7 +981,7 @@
       <c r="J21" s="15"/>
       <c r="K21" s="28"/>
     </row>
-    <row r="22" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+    <row r="22" spans="2:11" s="7" customFormat="1" ht="15">
       <c r="B22" s="28"/>
       <c r="D22" s="15"/>
       <c r="E22" s="28"/>
@@ -990,7 +990,7 @@
       <c r="J22" s="15"/>
       <c r="K22" s="28"/>
     </row>
-    <row r="23" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+    <row r="23" spans="2:11" s="7" customFormat="1" ht="15">
       <c r="B23" s="28"/>
       <c r="D23" s="15"/>
       <c r="E23" s="28"/>
@@ -999,7 +999,7 @@
       <c r="J23" s="15"/>
       <c r="K23" s="28"/>
     </row>
-    <row r="24" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+    <row r="24" spans="2:11" s="7" customFormat="1" ht="15">
       <c r="B24" s="28"/>
       <c r="D24" s="15"/>
       <c r="E24" s="28"/>
@@ -1008,7 +1008,7 @@
       <c r="J24" s="15"/>
       <c r="K24" s="28"/>
     </row>
-    <row r="25" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+    <row r="25" spans="2:11" s="7" customFormat="1" ht="15">
       <c r="B25" s="28"/>
       <c r="D25" s="15"/>
       <c r="E25" s="28"/>
@@ -1017,7 +1017,7 @@
       <c r="J25" s="15"/>
       <c r="K25" s="28"/>
     </row>
-    <row r="26" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+    <row r="26" spans="2:11" s="7" customFormat="1" ht="15">
       <c r="B26" s="28"/>
       <c r="D26" s="15"/>
       <c r="E26" s="28"/>
@@ -1026,7 +1026,7 @@
       <c r="J26" s="15"/>
       <c r="K26" s="28"/>
     </row>
-    <row r="27" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+    <row r="27" spans="2:11" s="7" customFormat="1" ht="15">
       <c r="B27" s="28"/>
       <c r="D27" s="15"/>
       <c r="E27" s="28"/>
@@ -1035,7 +1035,7 @@
       <c r="J27" s="15"/>
       <c r="K27" s="28"/>
     </row>
-    <row r="28" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+    <row r="28" spans="2:11" s="7" customFormat="1" ht="15">
       <c r="B28" s="28"/>
       <c r="D28" s="15"/>
       <c r="E28" s="28"/>
@@ -1044,7 +1044,7 @@
       <c r="J28" s="15"/>
       <c r="K28" s="28"/>
     </row>
-    <row r="29" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+    <row r="29" spans="2:11" s="7" customFormat="1" ht="15">
       <c r="B29" s="28"/>
       <c r="D29" s="15"/>
       <c r="E29" s="28"/>
@@ -1053,7 +1053,7 @@
       <c r="J29" s="15"/>
       <c r="K29" s="28"/>
     </row>
-    <row r="30" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+    <row r="30" spans="2:11" s="7" customFormat="1" ht="15">
       <c r="B30" s="28"/>
       <c r="D30" s="15"/>
       <c r="E30" s="28"/>
@@ -1062,7 +1062,7 @@
       <c r="J30" s="15"/>
       <c r="K30" s="28"/>
     </row>
-    <row r="31" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+    <row r="31" spans="2:11" s="7" customFormat="1" ht="15">
       <c r="B31" s="28"/>
       <c r="D31" s="15"/>
       <c r="E31" s="28"/>
@@ -1071,7 +1071,7 @@
       <c r="J31" s="15"/>
       <c r="K31" s="28"/>
     </row>
-    <row r="32" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+    <row r="32" spans="2:11" s="7" customFormat="1" ht="15">
       <c r="B32" s="28"/>
       <c r="D32" s="15"/>
       <c r="E32" s="28"/>
@@ -1080,7 +1080,7 @@
       <c r="J32" s="15"/>
       <c r="K32" s="28"/>
     </row>
-    <row r="33" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+    <row r="33" spans="2:11" s="7" customFormat="1" ht="15">
       <c r="B33" s="28"/>
       <c r="D33" s="15"/>
       <c r="E33" s="28"/>
@@ -1089,7 +1089,7 @@
       <c r="J33" s="15"/>
       <c r="K33" s="28"/>
     </row>
-    <row r="34" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+    <row r="34" spans="2:11" s="7" customFormat="1" ht="15">
       <c r="B34" s="28"/>
       <c r="D34" s="15"/>
       <c r="E34" s="28"/>
@@ -1098,7 +1098,7 @@
       <c r="J34" s="15"/>
       <c r="K34" s="28"/>
     </row>
-    <row r="35" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+    <row r="35" spans="2:11" s="7" customFormat="1" ht="15">
       <c r="B35" s="28"/>
       <c r="D35" s="15"/>
       <c r="E35" s="28"/>
@@ -1107,7 +1107,7 @@
       <c r="J35" s="15"/>
       <c r="K35" s="28"/>
     </row>
-    <row r="36" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+    <row r="36" spans="2:11" s="7" customFormat="1" ht="15">
       <c r="B36" s="28"/>
       <c r="D36" s="15"/>
       <c r="E36" s="28"/>
@@ -1116,7 +1116,7 @@
       <c r="J36" s="15"/>
       <c r="K36" s="28"/>
     </row>
-    <row r="37" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+    <row r="37" spans="2:11" s="7" customFormat="1" ht="15">
       <c r="B37" s="28"/>
       <c r="D37" s="15"/>
       <c r="E37" s="28"/>
@@ -1125,7 +1125,7 @@
       <c r="J37" s="15"/>
       <c r="K37" s="28"/>
     </row>
-    <row r="38" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+    <row r="38" spans="2:11" s="7" customFormat="1" ht="15">
       <c r="B38" s="28"/>
       <c r="D38" s="15"/>
       <c r="E38" s="28"/>
@@ -1134,7 +1134,7 @@
       <c r="J38" s="15"/>
       <c r="K38" s="28"/>
     </row>
-    <row r="39" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+    <row r="39" spans="2:11" s="7" customFormat="1" ht="15">
       <c r="B39" s="28"/>
       <c r="D39" s="15"/>
       <c r="E39" s="28"/>
@@ -1143,7 +1143,7 @@
       <c r="J39" s="15"/>
       <c r="K39" s="28"/>
     </row>
-    <row r="40" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+    <row r="40" spans="2:11" s="7" customFormat="1" ht="15">
       <c r="B40" s="28"/>
       <c r="D40" s="15"/>
       <c r="E40" s="28"/>
@@ -1152,7 +1152,7 @@
       <c r="J40" s="15"/>
       <c r="K40" s="28"/>
     </row>
-    <row r="41" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+    <row r="41" spans="2:11" s="7" customFormat="1" ht="15">
       <c r="B41" s="28"/>
       <c r="D41" s="15"/>
       <c r="E41" s="28"/>
@@ -1161,7 +1161,7 @@
       <c r="J41" s="15"/>
       <c r="K41" s="28"/>
     </row>
-    <row r="42" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+    <row r="42" spans="2:11" s="7" customFormat="1" ht="15">
       <c r="B42" s="28"/>
       <c r="D42" s="15"/>
       <c r="E42" s="28"/>
@@ -1170,7 +1170,7 @@
       <c r="J42" s="15"/>
       <c r="K42" s="28"/>
     </row>
-    <row r="43" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+    <row r="43" spans="2:11" s="7" customFormat="1" ht="15">
       <c r="B43" s="28"/>
       <c r="D43" s="15"/>
       <c r="E43" s="28"/>
@@ -1179,7 +1179,7 @@
       <c r="J43" s="15"/>
       <c r="K43" s="28"/>
     </row>
-    <row r="44" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+    <row r="44" spans="2:11" s="7" customFormat="1" ht="15">
       <c r="B44" s="28"/>
       <c r="D44" s="15"/>
       <c r="E44" s="28"/>
@@ -1188,7 +1188,7 @@
       <c r="J44" s="15"/>
       <c r="K44" s="28"/>
     </row>
-    <row r="45" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
+    <row r="45" spans="2:11" s="7" customFormat="1" ht="15">
       <c r="B45" s="28"/>
       <c r="D45" s="15"/>
       <c r="E45" s="28"/>

</xml_diff>

<commit_message>
Translated buttons, fixed instructions, skipphases
Co-Authored-By: Haifeng Zhao <24635433+hyphenzhao@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/0_Instructions.xlsx
+++ b/0_Instructions.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="338" documentId="13_ncr:1_{1C5A802C-9E12-9642-81BF-202D7BBFE009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9381E74F-0363-42A2-82A4-50836C312F19}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E756B8-758B-4DF5-AA99-51838A8A289C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="31">
   <si>
     <t>You will see different faces appear on the screen. Please carefully observe them.</t>
   </si>
@@ -82,13 +82,7 @@
     <t>When you see the face below, please left-click the mouse as fast as you can</t>
   </si>
   <si>
-    <t>Before we continue, feel free to take a break of 5-10 minutes.</t>
-  </si>
-  <si>
     <t>同样，你会看到屏幕上出现不同的面孔。请仔细观察它们。</t>
-  </si>
-  <si>
-    <t>在我们继续之前，请放松地休息5-10分钟.</t>
   </si>
   <si>
     <t>测试结束，感谢您的参与！</t>
@@ -125,7 +119,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -354,10 +348,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -625,27 +615,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="17.7" x14ac:dyDescent="0.85"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="33.28515625" style="29" customWidth="1"/>
+    <col min="1" max="1" width="33.26171875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="33.26171875" style="29" customWidth="1"/>
     <col min="3" max="3" width="16" style="3" customWidth="1"/>
-    <col min="4" max="4" width="33.28515625" style="16" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" style="29" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="25.42578125" style="16" customWidth="1"/>
-    <col min="8" max="8" width="39.140625" style="29" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="23.85546875" style="16" customWidth="1"/>
+    <col min="4" max="4" width="33.26171875" style="16" customWidth="1"/>
+    <col min="5" max="5" width="30.26171875" style="29" customWidth="1"/>
+    <col min="6" max="6" width="12.578125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="25.41796875" style="16" customWidth="1"/>
+    <col min="8" max="8" width="39.15625" style="29" customWidth="1"/>
+    <col min="9" max="9" width="15.15625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="23.83984375" style="16" customWidth="1"/>
     <col min="11" max="11" width="26" style="29" customWidth="1"/>
-    <col min="12" max="16384" width="8.85546875" style="3"/>
+    <col min="12" max="16384" width="8.83984375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="37.5">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="36.6" x14ac:dyDescent="0.7">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -680,42 +670,42 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="60" customHeight="1">
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>18</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H2" s="30" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I2" s="19" t="s">
         <v>18</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="K2" s="23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="14" customFormat="1" ht="84" customHeight="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="14" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.8">
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
@@ -729,16 +719,16 @@
         <v>9</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>18</v>
       </c>
       <c r="G3" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="26" t="s">
         <v>20</v>
-      </c>
-      <c r="H3" s="26" t="s">
-        <v>22</v>
       </c>
       <c r="I3" s="8" t="s">
         <v>18</v>
@@ -746,12 +736,12 @@
       <c r="J3" s="20"/>
       <c r="K3" s="27"/>
     </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" ht="48" customHeight="1">
+    <row r="4" spans="1:11" s="1" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.8">
       <c r="A4" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>15</v>
@@ -760,60 +750,60 @@
         <v>19</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F4" s="19" t="s">
         <v>15</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="H4" s="25" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="I4" s="19" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J4" s="22"/>
       <c r="K4" s="31"/>
     </row>
-    <row r="5" spans="1:11" s="14" customFormat="1" ht="63">
+    <row r="5" spans="1:11" s="14" customFormat="1" ht="35.4" x14ac:dyDescent="0.8">
       <c r="A5" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="H5" s="24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="J5" s="20"/>
       <c r="K5" s="27"/>
     </row>
-    <row r="6" spans="1:11" s="1" customFormat="1" ht="59.1" customHeight="1">
+    <row r="6" spans="1:11" s="1" customFormat="1" ht="59.1" customHeight="1" x14ac:dyDescent="0.8">
       <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C6" s="19" t="s">
         <v>18</v>
@@ -822,40 +812,34 @@
         <v>13</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F6" s="19" t="s">
         <v>18</v>
       </c>
       <c r="G6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="23" t="s">
-        <v>31</v>
-      </c>
       <c r="I6" s="4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="J6" s="22"/>
       <c r="K6" s="31"/>
     </row>
-    <row r="7" spans="1:11" s="12" customFormat="1" ht="69.599999999999994" customHeight="1">
+    <row r="7" spans="1:11" s="12" customFormat="1" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.8">
       <c r="B7" s="27"/>
       <c r="D7" s="20"/>
       <c r="E7" s="27"/>
-      <c r="G7" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>18</v>
-      </c>
+      <c r="G7" s="17"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="10"/>
       <c r="J7" s="20"/>
       <c r="K7" s="27"/>
     </row>
-    <row r="8" spans="1:11" s="7" customFormat="1" ht="15">
+    <row r="8" spans="1:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
       <c r="B8" s="28"/>
       <c r="D8" s="15"/>
       <c r="E8" s="28"/>
@@ -864,7 +848,7 @@
       <c r="J8" s="15"/>
       <c r="K8" s="28"/>
     </row>
-    <row r="9" spans="1:11" s="7" customFormat="1" ht="15">
+    <row r="9" spans="1:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
       <c r="B9" s="28"/>
       <c r="D9" s="15"/>
       <c r="E9" s="28"/>
@@ -873,7 +857,7 @@
       <c r="J9" s="15"/>
       <c r="K9" s="28"/>
     </row>
-    <row r="10" spans="1:11" s="7" customFormat="1" ht="15">
+    <row r="10" spans="1:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
       <c r="B10" s="28"/>
       <c r="D10" s="15"/>
       <c r="E10" s="28"/>
@@ -882,7 +866,7 @@
       <c r="J10" s="15"/>
       <c r="K10" s="28"/>
     </row>
-    <row r="11" spans="1:11" s="7" customFormat="1">
+    <row r="11" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.85">
       <c r="B11" s="28"/>
       <c r="D11" s="15"/>
       <c r="E11" s="28"/>
@@ -891,7 +875,7 @@
       <c r="J11" s="15"/>
       <c r="K11" s="28"/>
     </row>
-    <row r="12" spans="1:11" s="7" customFormat="1" ht="15">
+    <row r="12" spans="1:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
       <c r="B12" s="28"/>
       <c r="D12" s="15"/>
       <c r="E12" s="28"/>
@@ -900,7 +884,7 @@
       <c r="J12" s="15"/>
       <c r="K12" s="28"/>
     </row>
-    <row r="13" spans="1:11" s="7" customFormat="1" ht="15">
+    <row r="13" spans="1:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
       <c r="B13" s="28"/>
       <c r="D13" s="15"/>
       <c r="E13" s="28"/>
@@ -909,7 +893,7 @@
       <c r="J13" s="15"/>
       <c r="K13" s="28"/>
     </row>
-    <row r="14" spans="1:11" s="7" customFormat="1" ht="15">
+    <row r="14" spans="1:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
       <c r="B14" s="28"/>
       <c r="D14" s="15"/>
       <c r="E14" s="28"/>
@@ -918,7 +902,7 @@
       <c r="J14" s="15"/>
       <c r="K14" s="28"/>
     </row>
-    <row r="15" spans="1:11" s="7" customFormat="1" ht="15">
+    <row r="15" spans="1:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
       <c r="B15" s="28"/>
       <c r="D15" s="15"/>
       <c r="E15" s="28"/>
@@ -927,7 +911,7 @@
       <c r="J15" s="15"/>
       <c r="K15" s="28"/>
     </row>
-    <row r="16" spans="1:11" s="7" customFormat="1" ht="15">
+    <row r="16" spans="1:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
       <c r="B16" s="28"/>
       <c r="D16" s="15"/>
       <c r="E16" s="28"/>
@@ -936,7 +920,7 @@
       <c r="J16" s="15"/>
       <c r="K16" s="28"/>
     </row>
-    <row r="17" spans="2:11" s="7" customFormat="1" ht="15">
+    <row r="17" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
       <c r="B17" s="28"/>
       <c r="D17" s="15"/>
       <c r="E17" s="28"/>
@@ -945,7 +929,7 @@
       <c r="J17" s="15"/>
       <c r="K17" s="28"/>
     </row>
-    <row r="18" spans="2:11" s="7" customFormat="1" ht="15">
+    <row r="18" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
       <c r="B18" s="28"/>
       <c r="D18" s="15"/>
       <c r="E18" s="28"/>
@@ -954,7 +938,7 @@
       <c r="J18" s="15"/>
       <c r="K18" s="28"/>
     </row>
-    <row r="19" spans="2:11" s="7" customFormat="1" ht="15">
+    <row r="19" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
       <c r="B19" s="28"/>
       <c r="D19" s="15"/>
       <c r="E19" s="28"/>
@@ -963,7 +947,7 @@
       <c r="J19" s="15"/>
       <c r="K19" s="28"/>
     </row>
-    <row r="20" spans="2:11" s="7" customFormat="1" ht="15">
+    <row r="20" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
       <c r="B20" s="28"/>
       <c r="D20" s="15"/>
       <c r="E20" s="28"/>
@@ -972,7 +956,7 @@
       <c r="J20" s="15"/>
       <c r="K20" s="28"/>
     </row>
-    <row r="21" spans="2:11" s="7" customFormat="1" ht="15">
+    <row r="21" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
       <c r="B21" s="28"/>
       <c r="D21" s="15"/>
       <c r="E21" s="28"/>
@@ -981,7 +965,7 @@
       <c r="J21" s="15"/>
       <c r="K21" s="28"/>
     </row>
-    <row r="22" spans="2:11" s="7" customFormat="1" ht="15">
+    <row r="22" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
       <c r="B22" s="28"/>
       <c r="D22" s="15"/>
       <c r="E22" s="28"/>
@@ -990,7 +974,7 @@
       <c r="J22" s="15"/>
       <c r="K22" s="28"/>
     </row>
-    <row r="23" spans="2:11" s="7" customFormat="1" ht="15">
+    <row r="23" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
       <c r="B23" s="28"/>
       <c r="D23" s="15"/>
       <c r="E23" s="28"/>
@@ -999,7 +983,7 @@
       <c r="J23" s="15"/>
       <c r="K23" s="28"/>
     </row>
-    <row r="24" spans="2:11" s="7" customFormat="1" ht="15">
+    <row r="24" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
       <c r="B24" s="28"/>
       <c r="D24" s="15"/>
       <c r="E24" s="28"/>
@@ -1008,7 +992,7 @@
       <c r="J24" s="15"/>
       <c r="K24" s="28"/>
     </row>
-    <row r="25" spans="2:11" s="7" customFormat="1" ht="15">
+    <row r="25" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
       <c r="B25" s="28"/>
       <c r="D25" s="15"/>
       <c r="E25" s="28"/>
@@ -1017,7 +1001,7 @@
       <c r="J25" s="15"/>
       <c r="K25" s="28"/>
     </row>
-    <row r="26" spans="2:11" s="7" customFormat="1" ht="15">
+    <row r="26" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
       <c r="B26" s="28"/>
       <c r="D26" s="15"/>
       <c r="E26" s="28"/>
@@ -1026,7 +1010,7 @@
       <c r="J26" s="15"/>
       <c r="K26" s="28"/>
     </row>
-    <row r="27" spans="2:11" s="7" customFormat="1" ht="15">
+    <row r="27" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
       <c r="B27" s="28"/>
       <c r="D27" s="15"/>
       <c r="E27" s="28"/>
@@ -1035,7 +1019,7 @@
       <c r="J27" s="15"/>
       <c r="K27" s="28"/>
     </row>
-    <row r="28" spans="2:11" s="7" customFormat="1" ht="15">
+    <row r="28" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
       <c r="B28" s="28"/>
       <c r="D28" s="15"/>
       <c r="E28" s="28"/>
@@ -1044,7 +1028,7 @@
       <c r="J28" s="15"/>
       <c r="K28" s="28"/>
     </row>
-    <row r="29" spans="2:11" s="7" customFormat="1" ht="15">
+    <row r="29" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
       <c r="B29" s="28"/>
       <c r="D29" s="15"/>
       <c r="E29" s="28"/>
@@ -1053,7 +1037,7 @@
       <c r="J29" s="15"/>
       <c r="K29" s="28"/>
     </row>
-    <row r="30" spans="2:11" s="7" customFormat="1" ht="15">
+    <row r="30" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
       <c r="B30" s="28"/>
       <c r="D30" s="15"/>
       <c r="E30" s="28"/>
@@ -1062,7 +1046,7 @@
       <c r="J30" s="15"/>
       <c r="K30" s="28"/>
     </row>
-    <row r="31" spans="2:11" s="7" customFormat="1" ht="15">
+    <row r="31" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
       <c r="B31" s="28"/>
       <c r="D31" s="15"/>
       <c r="E31" s="28"/>
@@ -1071,7 +1055,7 @@
       <c r="J31" s="15"/>
       <c r="K31" s="28"/>
     </row>
-    <row r="32" spans="2:11" s="7" customFormat="1" ht="15">
+    <row r="32" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
       <c r="B32" s="28"/>
       <c r="D32" s="15"/>
       <c r="E32" s="28"/>
@@ -1080,7 +1064,7 @@
       <c r="J32" s="15"/>
       <c r="K32" s="28"/>
     </row>
-    <row r="33" spans="2:11" s="7" customFormat="1" ht="15">
+    <row r="33" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
       <c r="B33" s="28"/>
       <c r="D33" s="15"/>
       <c r="E33" s="28"/>
@@ -1089,7 +1073,7 @@
       <c r="J33" s="15"/>
       <c r="K33" s="28"/>
     </row>
-    <row r="34" spans="2:11" s="7" customFormat="1" ht="15">
+    <row r="34" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
       <c r="B34" s="28"/>
       <c r="D34" s="15"/>
       <c r="E34" s="28"/>
@@ -1098,7 +1082,7 @@
       <c r="J34" s="15"/>
       <c r="K34" s="28"/>
     </row>
-    <row r="35" spans="2:11" s="7" customFormat="1" ht="15">
+    <row r="35" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
       <c r="B35" s="28"/>
       <c r="D35" s="15"/>
       <c r="E35" s="28"/>
@@ -1107,7 +1091,7 @@
       <c r="J35" s="15"/>
       <c r="K35" s="28"/>
     </row>
-    <row r="36" spans="2:11" s="7" customFormat="1" ht="15">
+    <row r="36" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
       <c r="B36" s="28"/>
       <c r="D36" s="15"/>
       <c r="E36" s="28"/>
@@ -1116,7 +1100,7 @@
       <c r="J36" s="15"/>
       <c r="K36" s="28"/>
     </row>
-    <row r="37" spans="2:11" s="7" customFormat="1" ht="15">
+    <row r="37" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
       <c r="B37" s="28"/>
       <c r="D37" s="15"/>
       <c r="E37" s="28"/>
@@ -1125,7 +1109,7 @@
       <c r="J37" s="15"/>
       <c r="K37" s="28"/>
     </row>
-    <row r="38" spans="2:11" s="7" customFormat="1" ht="15">
+    <row r="38" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
       <c r="B38" s="28"/>
       <c r="D38" s="15"/>
       <c r="E38" s="28"/>
@@ -1134,7 +1118,7 @@
       <c r="J38" s="15"/>
       <c r="K38" s="28"/>
     </row>
-    <row r="39" spans="2:11" s="7" customFormat="1" ht="15">
+    <row r="39" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
       <c r="B39" s="28"/>
       <c r="D39" s="15"/>
       <c r="E39" s="28"/>
@@ -1143,7 +1127,7 @@
       <c r="J39" s="15"/>
       <c r="K39" s="28"/>
     </row>
-    <row r="40" spans="2:11" s="7" customFormat="1" ht="15">
+    <row r="40" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
       <c r="B40" s="28"/>
       <c r="D40" s="15"/>
       <c r="E40" s="28"/>
@@ -1152,7 +1136,7 @@
       <c r="J40" s="15"/>
       <c r="K40" s="28"/>
     </row>
-    <row r="41" spans="2:11" s="7" customFormat="1" ht="15">
+    <row r="41" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
       <c r="B41" s="28"/>
       <c r="D41" s="15"/>
       <c r="E41" s="28"/>
@@ -1161,7 +1145,7 @@
       <c r="J41" s="15"/>
       <c r="K41" s="28"/>
     </row>
-    <row r="42" spans="2:11" s="7" customFormat="1" ht="15">
+    <row r="42" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
       <c r="B42" s="28"/>
       <c r="D42" s="15"/>
       <c r="E42" s="28"/>
@@ -1170,7 +1154,7 @@
       <c r="J42" s="15"/>
       <c r="K42" s="28"/>
     </row>
-    <row r="43" spans="2:11" s="7" customFormat="1" ht="15">
+    <row r="43" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
       <c r="B43" s="28"/>
       <c r="D43" s="15"/>
       <c r="E43" s="28"/>
@@ -1179,7 +1163,7 @@
       <c r="J43" s="15"/>
       <c r="K43" s="28"/>
     </row>
-    <row r="44" spans="2:11" s="7" customFormat="1" ht="15">
+    <row r="44" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
       <c r="B44" s="28"/>
       <c r="D44" s="15"/>
       <c r="E44" s="28"/>
@@ -1188,7 +1172,7 @@
       <c r="J44" s="15"/>
       <c r="K44" s="28"/>
     </row>
-    <row r="45" spans="2:11" s="7" customFormat="1" ht="15">
+    <row r="45" spans="2:11" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.8">
       <c r="B45" s="28"/>
       <c r="D45" s="15"/>
       <c r="E45" s="28"/>

</xml_diff>